<commit_message>
clear video files and update milestone
</commit_message>
<xml_diff>
--- a/milestone.xlsx
+++ b/milestone.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuanhengmu/Dokumente/DCAITI_Projekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuanhengmu/Dropbox/DCAITI_Vertief_PJ/Pre 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8570D155-93C8-FF44-B83B-64143A06FF8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A41B030-C4CB-154C-BB28-34D2BCB24AD0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>3rd Pre.</t>
   </si>
   <si>
-    <t>2nd Meeting</t>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -64,7 +64,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -126,8 +126,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -148,13 +155,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB1FF5F"/>
         <bgColor rgb="FF008080"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
@@ -188,7 +207,7 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -196,26 +215,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -225,6 +234,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Excel Built-in Accent2" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
@@ -300,6 +326,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFB1FF5F"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -609,10 +638,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
@@ -626,9 +655,10 @@
     <col min="7" max="7" width="28" customWidth="1"/>
     <col min="8" max="8" width="25.33203125" customWidth="1"/>
     <col min="9" max="9" width="8.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -641,10 +671,10 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -656,101 +686,109 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="2">
         <v>47</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="9"/>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="2">
         <v>48</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="2">
         <v>49</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="10"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2">
         <v>50</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="10"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="2">
         <v>51</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="2">
         <v>52</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="13"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="2">
         <v>53</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="E8" s="10"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -758,14 +796,15 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="10">
+      <c r="F9" s="6">
         <v>44202</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="G9" s="9"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -774,11 +813,12 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="G10" s="10"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="9"/>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -787,11 +827,12 @@
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="1:9">
+      <c r="G11" s="10"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="9"/>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="2">
         <v>4</v>
       </c>
@@ -801,10 +842,11 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="1:9">
+      <c r="H12" s="10"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="2">
         <v>5</v>
       </c>
@@ -814,10 +856,11 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="1:9">
+      <c r="H13" s="10"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="2">
         <v>6</v>
       </c>
@@ -827,19 +870,69 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="7">
+      <c r="H14" s="2"/>
+      <c r="I14" s="5">
         <v>44237</v>
       </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="8"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="13">
+        <v>7</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="15"/>
+    </row>
+    <row r="16" spans="1:10">
+      <c r="A16" s="16">
+        <v>8</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="15"/>
+    </row>
+    <row r="17" spans="1:10">
+      <c r="A17" s="16">
+        <v>9</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="15"/>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="16">
+        <v>10</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="11">
+        <v>44265</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>